<commit_message>
Correction Create_Language auto évolution de la langue add readme.MD Trieur suppression de la def rectiftieur
</commit_message>
<xml_diff>
--- a/Createur/New_File2.xlsx
+++ b/Createur/New_File2.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -424,12 +424,912 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
+          <t>contiennent</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>contener</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>contient</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>contiene</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>continent</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>continente</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>continental</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>continental</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>continentale</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>continental</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>continents</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>continentes</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>contingences</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>contingencias</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>contingent</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>contingente</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>continu</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>continuar</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>continuaient</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>continuado</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>continuait</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>continuado</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>continuant</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>continuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>continuateur</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>continuador</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>continue</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>continuar</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>continuel</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>continuo</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>continuellement</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>continuamente</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>continuent</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>continuar</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>continuer</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>seguir</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>continuera</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>continuar a</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>continuerait</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>continuaría</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>continueront</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>continuará</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>continuite</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>continuar</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>contorsion</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>contorsión</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>contour</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>contorno</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>contourner</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>llegar</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>contours</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>contornos</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>contraceptif</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>anticonceptivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>contractee</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>contratista</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>contracter</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>contraer</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>contraction</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>contracción</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>contractuelle</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>contractual</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>contradiction</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>contradicción</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>contradictions</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>contradicciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>contradictoire</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>contradictorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>contradictoires</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>contradictorio</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>contraignant</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>restrictivo</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>contraignante</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>vinculante</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>contraignantes</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>vinculante</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>contraindre</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>constreñir</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>contraint</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>constreñido</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>contrainte</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>restricción</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>contraintes</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>restricciones</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>contraints</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>forzado</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>contraire</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>opuesto</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>consulaire</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>консулски</t>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>de cónsul</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>contrairement</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>contrariamente a</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>contraires</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>opuestos</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>contralto</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>contralto</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>contrariant</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>irritante</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>contrarie</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>contrario</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>contrarier</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>enojarse</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>contrariete</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>no estarás de acuerdo</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>contrario</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>contrario</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>contraste</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>contraste</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>contraster</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>contraste</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>contrat</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>CONTRATO</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>contrats</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>contratos</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>contravention</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>contravención</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>contre</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>contra</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>contrebalancer</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>contrapeso</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>contrebande</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>contrabando</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>contrecarrer</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>frustrar</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>contrecoeur</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>de mala gana</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>contrecoup</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>reacción</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>contredire</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>contradecir</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>contredit</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>contradijo</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>contree</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>contra</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>contrefacon</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>contrafacón</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>contrefait</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>falsificación</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>contrepartie</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>consideración</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>contre-pied</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>contra pie</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>contrepoids</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>contrapeso</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>contrer</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>para contrarrestar</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>contribuable</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>contribuyente</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>contribuables</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>contribuyentes</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>contribuant</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>contribuyendo</t>
         </is>
       </c>
     </row>

</xml_diff>